<commit_message>
Update DateBase/orders/Dang Nguyen 195_2026-2-9.xlsx
</commit_message>
<xml_diff>
--- a/DateBase/orders/Dang Nguyen 195_2026-2-9.xlsx
+++ b/DateBase/orders/Dang Nguyen 195_2026-2-9.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -877,12 +877,101 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
+        <v>15</v>
+      </c>
+      <c r="C51" t="str">
+        <v>147_娜欧米_Red Naomi_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F51" t="str">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="C52" t="str">
+        <v>175_火灵鸟_Free Spirit_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F52" t="str">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="C53" t="str">
+        <v>203_佛罗伊德_Floyd_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F53" t="str">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="C54" t="str">
+        <v>411_紫罗兰白_violet white_undefined_1bunch</v>
+      </c>
+      <c r="F54" t="str">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>16</v>
+      </c>
+      <c r="C55" t="str">
+        <v>279_完美甜蜜_undefined_Rosa rugosa Thunb._10stems</v>
+      </c>
+      <c r="F55" t="str">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="C56" t="str">
+        <v>144_高原红_High Plateau Red_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F56" t="str">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="C57" t="str">
+        <v>412_紫罗兰粉_violet pink_undefined_1bunch</v>
+      </c>
+      <c r="F57" t="str">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>17</v>
+      </c>
+      <c r="C58" t="str">
+        <v>144_高原红_High Plateau Red_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F58" t="str">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="C59" t="str">
+        <v>203_佛罗伊德_Floyd_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F59" t="str">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="C60" t="str">
+        <v>412_紫罗兰粉_violet pink_undefined_1bunch</v>
+      </c>
+      <c r="F60" t="str">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L51"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L61"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -940,7 +1029,7 @@
         <v>0.00</v>
       </c>
       <c r="G2" t="str">
-        <v>03014531467109145105338405302055501059570301001030738510121551542030101530312101050</v>
+        <v>03014531467109145105338405302055501059570301001030738510121551542030101530312101051747.5201527101818100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>